<commit_message>
Removed P/p issue from publication type (two different forms of the word)
</commit_message>
<xml_diff>
--- a/docs/publication/publication-metadata.xlsx
+++ b/docs/publication/publication-metadata.xlsx
@@ -78,7 +78,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="7" uniqueCount="7">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="6" uniqueCount="6">
   <si>
     <t>version</t>
   </si>
@@ -87,9 +87,6 @@
   </si>
   <si>
     <t>assay_type</t>
-  </si>
-  <si>
-    <t>Publication</t>
   </si>
   <si>
     <t>publication</t>
@@ -464,10 +461,10 @@
         <v>2</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="D1" s="1" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
     </row>
   </sheetData>
@@ -475,8 +472,8 @@
     <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" errorTitle="Value must come from list" error="Value must be one of: 0." sqref="A2:A1048576">
       <formula1>'version list'!$A$1:$A$1</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" errorTitle="Value must come from list" error="Value must be one of: Publication / publication." sqref="B2:B1048576">
-      <formula1>'assay_type list'!$A$1:$A$2</formula1>
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" errorTitle="Value must come from list" error="Value must be one of: publication." sqref="B2:B1048576">
+      <formula1>'assay_type list'!$A$1:$A$1</formula1>
     </dataValidation>
   </dataValidations>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -504,7 +501,7 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:A2"/>
+  <dimension ref="A1"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
@@ -515,11 +512,6 @@
         <v>3</v>
       </c>
     </row>
-    <row r="2" spans="1:1">
-      <c r="A2" t="s">
-        <v>4</v>
-      </c>
-    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
Removed P/p issue from publication type (two different forms of the word) (#1195)
</commit_message>
<xml_diff>
--- a/docs/publication/publication-metadata.xlsx
+++ b/docs/publication/publication-metadata.xlsx
@@ -78,7 +78,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="7" uniqueCount="7">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="6" uniqueCount="6">
   <si>
     <t>version</t>
   </si>
@@ -87,9 +87,6 @@
   </si>
   <si>
     <t>assay_type</t>
-  </si>
-  <si>
-    <t>Publication</t>
   </si>
   <si>
     <t>publication</t>
@@ -464,10 +461,10 @@
         <v>2</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="D1" s="1" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
     </row>
   </sheetData>
@@ -475,8 +472,8 @@
     <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" errorTitle="Value must come from list" error="Value must be one of: 0." sqref="A2:A1048576">
       <formula1>'version list'!$A$1:$A$1</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" errorTitle="Value must come from list" error="Value must be one of: Publication / publication." sqref="B2:B1048576">
-      <formula1>'assay_type list'!$A$1:$A$2</formula1>
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" errorTitle="Value must come from list" error="Value must be one of: publication." sqref="B2:B1048576">
+      <formula1>'assay_type list'!$A$1:$A$1</formula1>
     </dataValidation>
   </dataValidations>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -504,7 +501,7 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:A2"/>
+  <dimension ref="A1"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
@@ -515,11 +512,6 @@
         <v>3</v>
       </c>
     </row>
-    <row r="2" spans="1:1">
-      <c r="A2" t="s">
-        <v>4</v>
-      </c>
-    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>